<commit_message>
da sua dc loi xoa lich hoc
</commit_message>
<xml_diff>
--- a/file/datalichhoc.xlsx
+++ b/file/datalichhoc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VisualStudioCode\data_baitaplon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA3B5CC4-0066-471B-BB96-0C3B30B511BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14FB9A0-45AC-41C3-AFEB-38EB84982505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,12 +48,6 @@
     <t>Ngày bắt đầu</t>
   </si>
   <si>
-    <t>Thực Hành 1</t>
-  </si>
-  <si>
-    <t>Thực Hành 2</t>
-  </si>
-  <si>
     <t>LHP51</t>
   </si>
   <si>
@@ -75,9 +69,6 @@
     <t>2020-12-08</t>
   </si>
   <si>
-    <t>Lý Thuyết</t>
-  </si>
-  <si>
     <t>07-10</t>
   </si>
   <si>
@@ -88,6 +79,15 @@
   </si>
   <si>
     <t>2020-12-09</t>
+  </si>
+  <si>
+    <t>TH1</t>
+  </si>
+  <si>
+    <t>TH2</t>
+  </si>
+  <si>
+    <t>LT</t>
   </si>
 </sst>
 </file>
@@ -415,7 +415,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -454,71 +454,71 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
       <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>